<commit_message>
createReport => add new update(fixed)
</commit_message>
<xml_diff>
--- a/src/public/25.01.2024.xlsx
+++ b/src/public/25.01.2024.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rufat\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462A4676-AFFB-43FA-8837-2FB73D420982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>№</t>
   </si>
@@ -41,12 +40,18 @@
   </si>
   <si>
     <t>Samir Rustamzada</t>
+  </si>
+  <si>
+    <t>Neman Ismiyev</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -139,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -154,7 +159,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -366,25 +371,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,12 +409,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>5183742</v>
+        <v>123321</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -422,6 +427,26 @@
       </c>
       <c r="F2" s="4">
         <v>239.46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5363124</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4">
+        <v>134.15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all support message  and admin will send message to user
</commit_message>
<xml_diff>
--- a/src/public/25.01.2024.xlsx
+++ b/src/public/25.01.2024.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>123321</v>
+        <v>123555</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>

</xml_diff>